<commit_message>
Finish and test the Naiv Bayes
</commit_message>
<xml_diff>
--- a/Projeto 2/Coca_Cola.xlsx
+++ b/Projeto 2/Coca_Cola.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="407">
   <si>
     <t>Treinamento</t>
   </si>
@@ -1293,6 +1293,9 @@
   </si>
   <si>
     <t>Relevancia</t>
+  </si>
+  <si>
+    <t>Relevancia_Pessoa</t>
   </si>
 </sst>
 </file>
@@ -1351,9 +1354,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1696,8 +1702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B301"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4121,1018 +4127,1628 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A201"/>
+  <dimension ref="A1:B201"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="139" customWidth="1"/>
+    <col min="2" max="2" width="17.36328125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B1" s="2" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B30" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B31" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B32" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B33" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B34" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B35" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B36" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B37" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B38" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B39" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B40" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B41" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B42" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B43" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B44" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B45" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B46" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B47" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B48" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B49" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B50" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B51" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B52" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B53" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B54" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B55" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B56" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B57" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B58" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B59" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B60" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B61" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B62" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B63" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B64" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B65" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B66" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B67" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B68" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B69" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B70" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B71" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B72" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B73" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B74" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B75" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B76" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B77" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B78" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B79" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B80" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B81" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B82" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B83" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B84" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B85" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B86" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B87" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B88" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B89" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B90" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B91" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B92" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B93" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B94" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B95" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B96" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B97" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B98" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B99" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B100" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B101" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B102" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B103" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B104" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B105" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B106" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B107" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B108" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B109" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B110" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B111" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B112" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B113" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B114" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B115" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B116" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B117" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B118" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B119" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B120" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B121" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B122" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B123" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B124" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B125" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B126" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B127" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B128" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B129" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B130" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B131" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B132" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B133" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B134" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B135" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B136" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B137" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B138" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B139" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B140" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B141" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B142" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B143" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B144" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B145" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B146" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B147" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B148" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B149" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B150" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B151" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B152" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B153" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B154" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B155" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B156" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B157" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B158" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B159" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B160" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B161" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B162" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B163" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B164" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B165" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B166" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B167" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B168" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B169" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B170" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B171" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B172" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B173" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B174" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B175" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B176" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B177" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B178" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B179" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B180" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B181" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B182" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B183" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B184" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B185" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B186" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B187" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B188" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B189" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B190" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B191" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B192" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B193" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B194" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B195" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B196" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B197" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B198" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B199" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B200" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>402</v>
       </c>
+      <c r="B201" t="s">
+        <v>403</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>